<commit_message>
commit -m "latest hybrid frame work with extent reports"
</commit_message>
<xml_diff>
--- a/Test_Data/Data_Provider.xlsx
+++ b/Test_Data/Data_Provider.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{008E6B48-FAC0-4AA7-A05E-CA37F70AFD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Email</t>
   </si>
@@ -43,13 +45,20 @@
   </si>
   <si>
     <t>mdzabi991@gmail.com</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,12 +74,22 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,11 +108,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -101,13 +124,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -145,7 +176,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -179,6 +210,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -213,9 +245,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -388,83 +421,98 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="21.88671875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
+      <c r="D1" t="s" s="0">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
+      <c r="D2" t="s" s="4">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>7</v>
       </c>
+      <c r="D3" t="s" s="5">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>7</v>
       </c>
+      <c r="D4" t="s" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>7</v>
+      </c>
+      <c r="D5" t="s" s="7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="A4" r:id="rId4"/>
-    <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="A5" r:id="rId6"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -472,24 +520,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
commit -m "CI-CD with latest Updates"
</commit_message>
<xml_diff>
--- a/Test_Data/Data_Provider.xlsx
+++ b/Test_Data/Data_Provider.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{008E6B48-FAC0-4AA7-A05E-CA37F70AFD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b621bfc7ae080d49/Documents/Telegram Desktop/selenium/hybrid/Hybrid_Framework/Test_Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:801_{008E6B48-FAC0-4AA7-A05E-CA37F70AFD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F18E7C3-D728-46D4-9459-C1811CDC7B3D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,12 +18,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Email</t>
   </si>
@@ -48,16 +52,12 @@
   </si>
   <si>
     <t>Result</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,22 +74,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,15 +98,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -430,22 +416,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="21.88671875"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0"/>
+    <col min="1" max="1" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -456,25 +442,19 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s" s="4">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -484,25 +464,19 @@
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" t="s" s="6">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" t="s" s="7">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit -m "to run bat file with jenkins"
</commit_message>
<xml_diff>
--- a/Test_Data/Data_Provider.xlsx
+++ b/Test_Data/Data_Provider.xlsx
@@ -3,12 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b621bfc7ae080d49/Documents/Telegram Desktop/selenium/hybrid/Hybrid_Framework/Test_Data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:801_{008E6B48-FAC0-4AA7-A05E-CA37F70AFD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F18E7C3-D728-46D4-9459-C1811CDC7B3D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D603481F-0236-45F4-97CE-53D901E51031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +13,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 

</xml_diff>

<commit_message>
commit -m "new changes"
</commit_message>
<xml_diff>
--- a/Test_Data/Data_Provider.xlsx
+++ b/Test_Data/Data_Provider.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D603481F-0236-45F4-97CE-53D901E51031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EECC05A5-35AE-4487-A8D9-07000358CD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Email</t>
   </si>
@@ -48,16 +48,12 @@
   </si>
   <si>
     <t>Result</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,22 +70,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,15 +94,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -425,27 +407,27 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="21.88671875"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0"/>
+    <col min="1" max="1" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -456,25 +438,19 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s" s="4">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -484,25 +460,19 @@
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" t="s" s="6">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" t="s" s="7">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit -m "new changes for testng"
</commit_message>
<xml_diff>
--- a/Test_Data/Data_Provider.xlsx
+++ b/Test_Data/Data_Provider.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EECC05A5-35AE-4487-A8D9-07000358CD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EF7BBCBD-4C65-409C-8B83-D763219AFD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>